<commit_message>
Turbulence model added Implementation of parallel processing on Experiment scripts. Working on Monitoring of results
</commit_message>
<xml_diff>
--- a/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
+++ b/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="39">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -128,28 +128,13 @@
     <t>Results</t>
   </si>
   <si>
-    <t>Unnamed: 7</t>
-  </si>
-  <si>
-    <t>Unnamed: 8</t>
-  </si>
-  <si>
-    <t>Unnamed: 9</t>
-  </si>
-  <si>
-    <t>Unnamed: 10</t>
-  </si>
-  <si>
-    <t>Unnamed: 11</t>
-  </si>
-  <si>
-    <t>Unnamed: 12</t>
-  </si>
-  <si>
     <t>Test #</t>
   </si>
   <si>
     <t>Crashed</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -1298,15 +1283,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>30</v>
@@ -1323,32 +1308,8 @@
       <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" s="1">
-        <v>0.666666666666667</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1362,13 +1323,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2">
-        <v>0.333333333333333</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1381,11 +1339,8 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1398,11 +1353,8 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1415,11 +1367,8 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1432,11 +1381,8 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1449,11 +1395,8 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1466,11 +1409,8 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1483,11 +1423,8 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1500,11 +1437,8 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1517,11 +1451,8 @@
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1534,11 +1465,8 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1551,11 +1479,8 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1568,11 +1493,8 @@
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1585,11 +1507,8 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1602,11 +1521,8 @@
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1619,11 +1535,8 @@
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="E17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1636,11 +1549,8 @@
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1653,11 +1563,8 @@
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1670,11 +1577,8 @@
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1687,11 +1591,8 @@
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1704,11 +1605,8 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1721,11 +1619,8 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1738,11 +1633,8 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1755,11 +1647,8 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="E25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1772,11 +1661,8 @@
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1789,11 +1675,8 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1806,11 +1689,8 @@
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1823,11 +1703,8 @@
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="E29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1840,11 +1717,8 @@
       <c r="D30">
         <v>1</v>
       </c>
-      <c r="E30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1857,11 +1731,8 @@
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1874,11 +1745,8 @@
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1891,11 +1759,8 @@
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="E33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1908,11 +1773,8 @@
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="E34" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1925,11 +1787,8 @@
       <c r="D35">
         <v>1</v>
       </c>
-      <c r="E35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1942,11 +1801,8 @@
       <c r="D36">
         <v>1</v>
       </c>
-      <c r="E36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1959,11 +1815,8 @@
       <c r="D37">
         <v>1</v>
       </c>
-      <c r="E37" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1976,11 +1829,8 @@
       <c r="D38">
         <v>1</v>
       </c>
-      <c r="E38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1994,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2008,7 +1858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2022,7 +1872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2036,7 +1886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2050,7 +1900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2064,7 +1914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:4">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2078,7 +1928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:4">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2092,7 +1942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:4">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2106,7 +1956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:4">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2317,7 +2167,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>30</v>
@@ -2345,6 +2195,9 @@
       <c r="D2">
         <v>0</v>
       </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
@@ -2359,6 +2212,9 @@
       <c r="D3">
         <v>0</v>
       </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
@@ -2373,6 +2229,9 @@
       <c r="D4">
         <v>0</v>
       </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1">
@@ -2387,6 +2246,9 @@
       <c r="D5">
         <v>0</v>
       </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1">
@@ -2400,6 +2262,9 @@
       </c>
       <c r="D6">
         <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2415,6 +2280,9 @@
       <c r="D7">
         <v>0</v>
       </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1">
@@ -2429,6 +2297,9 @@
       <c r="D8">
         <v>0</v>
       </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1">
@@ -2443,6 +2314,9 @@
       <c r="D9">
         <v>0</v>
       </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1">
@@ -2457,6 +2331,9 @@
       <c r="D10">
         <v>0</v>
       </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1">
@@ -2471,6 +2348,9 @@
       <c r="D11">
         <v>0</v>
       </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1">
@@ -2485,6 +2365,9 @@
       <c r="D12">
         <v>0</v>
       </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1">
@@ -2499,6 +2382,9 @@
       <c r="D13">
         <v>0</v>
       </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1">
@@ -2513,6 +2399,9 @@
       <c r="D14">
         <v>0</v>
       </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1">
@@ -2527,6 +2416,9 @@
       <c r="D15">
         <v>0</v>
       </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1">
@@ -2541,8 +2433,11 @@
       <c r="D16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2555,8 +2450,11 @@
       <c r="D17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2569,8 +2467,11 @@
       <c r="D18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2583,8 +2484,11 @@
       <c r="D19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2597,8 +2501,11 @@
       <c r="D20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2611,8 +2518,11 @@
       <c r="D21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2625,8 +2535,11 @@
       <c r="D22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2639,8 +2552,11 @@
       <c r="D23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2653,8 +2569,11 @@
       <c r="D24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2667,8 +2586,11 @@
       <c r="D25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2681,8 +2603,11 @@
       <c r="D26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2695,8 +2620,11 @@
       <c r="D27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2709,8 +2637,11 @@
       <c r="D28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2723,8 +2654,11 @@
       <c r="D29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2737,8 +2671,11 @@
       <c r="D30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2751,8 +2688,11 @@
       <c r="D31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2765,8 +2705,11 @@
       <c r="D32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2779,8 +2722,11 @@
       <c r="D33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2793,8 +2739,11 @@
       <c r="D34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2807,8 +2756,11 @@
       <c r="D35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2821,8 +2773,11 @@
       <c r="D36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2835,8 +2790,11 @@
       <c r="D37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2849,8 +2807,11 @@
       <c r="D38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2863,8 +2824,11 @@
       <c r="D39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2877,8 +2841,11 @@
       <c r="D40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2891,8 +2858,11 @@
       <c r="D41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2905,8 +2875,11 @@
       <c r="D42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2919,8 +2892,11 @@
       <c r="D43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2933,8 +2909,11 @@
       <c r="D44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2947,8 +2926,11 @@
       <c r="D45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2961,8 +2943,11 @@
       <c r="D46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2975,8 +2960,11 @@
       <c r="D47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2989,8 +2977,11 @@
       <c r="D48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3003,8 +2994,11 @@
       <c r="D49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3017,8 +3011,11 @@
       <c r="D50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3031,8 +3028,11 @@
       <c r="D51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3045,8 +3045,11 @@
       <c r="D52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3059,8 +3062,11 @@
       <c r="D53">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3073,8 +3079,11 @@
       <c r="D54">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3087,8 +3096,11 @@
       <c r="D55">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3101,8 +3113,11 @@
       <c r="D56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3115,8 +3130,11 @@
       <c r="D57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3129,8 +3147,11 @@
       <c r="D58">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3143,8 +3164,11 @@
       <c r="D59">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3157,8 +3181,11 @@
       <c r="D60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3170,6 +3197,9 @@
       </c>
       <c r="D61">
         <v>2</v>
+      </c>
+      <c r="E61" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working version on Serial processing, non-working on Parallel
</commit_message>
<xml_diff>
--- a/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
+++ b/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
@@ -131,10 +131,10 @@
     <t>Test #</t>
   </si>
   <si>
+    <t>Completed</t>
+  </si>
+  <si>
     <t>Crashed</t>
-  </si>
-  <si>
-    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -2196,7 +2196,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2213,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2230,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2247,7 +2247,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2264,7 +2264,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2281,7 +2281,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2298,7 +2298,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2315,7 +2315,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2332,7 +2332,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2349,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2366,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2383,7 +2383,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2400,7 +2400,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2417,7 +2417,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2434,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2451,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2468,7 +2468,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2485,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2502,7 +2502,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2519,7 +2519,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2536,7 +2536,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2553,7 +2553,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2570,7 +2570,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2587,7 +2587,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2604,7 +2604,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2621,7 +2621,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2638,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2655,7 +2655,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2672,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2689,7 +2689,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -2706,7 +2706,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2723,7 +2723,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2740,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2757,7 +2757,7 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2774,7 +2774,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -2791,7 +2791,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2808,7 +2808,7 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2825,7 +2825,7 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2842,7 +2842,7 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2859,7 +2859,7 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2876,7 +2876,7 @@
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2893,7 +2893,7 @@
         <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2910,7 +2910,7 @@
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2927,7 +2927,7 @@
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2944,7 +2944,7 @@
         <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2961,7 +2961,7 @@
         <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2978,7 +2978,7 @@
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2995,7 +2995,7 @@
         <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3012,7 +3012,7 @@
         <v>2</v>
       </c>
       <c r="E50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -3029,7 +3029,7 @@
         <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3046,7 +3046,7 @@
         <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3063,7 +3063,7 @@
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3080,7 +3080,7 @@
         <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3097,7 +3097,7 @@
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3114,7 +3114,7 @@
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3131,7 +3131,7 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3148,7 +3148,7 @@
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3165,7 +3165,7 @@
         <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3182,7 +3182,7 @@
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3199,7 +3199,7 @@
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update .gitignore, Unstable but working serial simulation
</commit_message>
<xml_diff>
--- a/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
+++ b/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
@@ -131,10 +131,10 @@
     <t>Test #</t>
   </si>
   <si>
+    <t>Crashed</t>
+  </si>
+  <si>
     <t>Completed</t>
-  </si>
-  <si>
-    <t>Crashed</t>
   </si>
 </sst>
 </file>
@@ -2196,7 +2196,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2213,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2230,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2247,7 +2247,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2264,7 +2264,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2281,7 +2281,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2298,7 +2298,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2315,7 +2315,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2332,7 +2332,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2349,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2366,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2383,7 +2383,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2400,7 +2400,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2417,7 +2417,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2434,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2451,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2468,7 +2468,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2485,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2502,7 +2502,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2519,7 +2519,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2536,7 +2536,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2553,7 +2553,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2570,7 +2570,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2587,7 +2587,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2604,7 +2604,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2621,7 +2621,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2638,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2655,7 +2655,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2672,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2689,7 +2689,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -2706,7 +2706,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2723,7 +2723,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2740,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2757,7 +2757,7 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2774,7 +2774,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -2791,7 +2791,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2808,7 +2808,7 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2825,7 +2825,7 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2842,7 +2842,7 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2859,7 +2859,7 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2876,7 +2876,7 @@
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2893,7 +2893,7 @@
         <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2910,7 +2910,7 @@
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2927,7 +2927,7 @@
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2944,7 +2944,7 @@
         <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2961,7 +2961,7 @@
         <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2978,7 +2978,7 @@
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2995,7 +2995,7 @@
         <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3012,7 +3012,7 @@
         <v>2</v>
       </c>
       <c r="E50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -3029,7 +3029,7 @@
         <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3046,7 +3046,7 @@
         <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3063,7 +3063,7 @@
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3080,7 +3080,7 @@
         <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3097,7 +3097,7 @@
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3114,7 +3114,7 @@
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3131,7 +3131,7 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3148,7 +3148,7 @@
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3165,7 +3165,7 @@
         <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3182,7 +3182,7 @@
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3199,7 +3199,7 @@
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed typo on nDTout at tempFlume
</commit_message>
<xml_diff>
--- a/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
+++ b/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="39">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -1465,6 +1465,9 @@
       <c r="D12">
         <v>0</v>
       </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1">

</xml_diff>

<commit_message>
Stable version with no reflective wave
</commit_message>
<xml_diff>
--- a/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
+++ b/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t xml:space="preserve">Unnamed: 0</t>
   </si>
@@ -134,7 +134,7 @@
     <t xml:space="preserve">Finished</t>
   </si>
   <si>
-    <t xml:space="preserve">Results</t>
+    <t xml:space="preserve">Time</t>
   </si>
   <si>
     <t xml:space="preserve">Completed</t>
@@ -1089,8 +1089,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1118,7 +1118,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -1131,11 +1131,8 @@
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
@@ -1148,11 +1145,8 @@
       <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
@@ -1165,11 +1159,8 @@
       <c r="D4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
@@ -1182,11 +1173,8 @@
       <c r="D5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
@@ -1214,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
@@ -1228,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
@@ -1242,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
@@ -1256,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
@@ -1270,7 +1258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
@@ -1284,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
@@ -1298,7 +1286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
@@ -1312,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
@@ -1326,7 +1314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
@@ -1340,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
@@ -1354,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
@@ -1368,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
@@ -1382,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
@@ -1396,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
@@ -1410,7 +1398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
@@ -1424,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
@@ -1438,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
@@ -1452,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
@@ -1466,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
@@ -1479,11 +1467,8 @@
       <c r="D26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E26" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
@@ -1497,7 +1482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
@@ -1511,7 +1496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
@@ -1761,6 +1746,12 @@
       </c>
       <c r="D46" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>20.0073922830283</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,7 +1980,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -2016,6 +2007,9 @@
       <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">

</xml_diff>

<commit_message>
Add interactive examples, dambreak_Colagrossi and broad_crested_weir
</commit_message>
<xml_diff>
--- a/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
+++ b/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="38">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>Completed</t>
-  </si>
-  <si>
-    <t>Crashed</t>
   </si>
 </sst>
 </file>
@@ -1326,7 +1323,7 @@
         <v>37</v>
       </c>
       <c r="F2">
-        <v>0.3100000000000001</v>
+        <v>60.01</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1343,10 +1340,10 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>15.01</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1809,6 +1806,12 @@
       </c>
       <c r="D36">
         <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36">
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:6">

</xml_diff>

<commit_message>
Debuggin Parallel script, problems with restart threads
</commit_message>
<xml_diff>
--- a/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
+++ b/2d/Interactive/Temp_Flume_GUI/DoE_TempFlume.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -41,6 +41,9 @@
     <t>Unnamed: 6</t>
   </si>
   <si>
+    <t>Unnamed: 7</t>
+  </si>
+  <si>
     <t>Scale 1/25</t>
   </si>
   <si>
@@ -105,6 +108,9 @@
   </si>
   <si>
     <t>mts</t>
+  </si>
+  <si>
+    <t>thickness in</t>
   </si>
   <si>
     <t>Levels</t>
@@ -489,13 +495,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,19 +523,25 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -539,44 +551,47 @@
       <c r="H3">
         <v>0.3048</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -594,12 +609,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>0.8</v>
@@ -617,12 +632,12 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>0.24384</v>
@@ -640,12 +655,12 @@
         <v>1.09728</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -660,12 +675,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>0.2</v>
@@ -680,12 +695,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>0.06096</v>
@@ -700,15 +715,15 @@
         <v>0.24384</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>0.5</v>
@@ -717,12 +732,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>0.006</v>
@@ -734,29 +749,29 @@
         <v>0.047</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14">
-        <v>0.0048288</v>
+        <v>0.0050038</v>
       </c>
       <c r="D14">
-        <v>0.0072672</v>
+        <v>0.0074422</v>
       </c>
       <c r="E14">
-        <v>0.0173256</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>0.0175006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -771,7 +786,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -779,22 +794,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -802,7 +817,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -825,7 +840,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C21">
         <v>0.872871560943969</v>
@@ -848,7 +863,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C22">
         <v>0.266051251775722</v>
@@ -871,7 +886,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -891,7 +906,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C24">
         <v>0.238095238095238</v>
@@ -911,7 +926,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25">
         <v>0.07257142857142861</v>
@@ -931,16 +946,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -948,7 +963,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C27">
         <v>0.005</v>
@@ -965,16 +980,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C28">
-        <v>0.004524</v>
+        <v>0.004699</v>
       </c>
       <c r="D28">
-        <v>0.006048</v>
+        <v>0.006223</v>
       </c>
       <c r="E28">
-        <v>0.0164112</v>
+        <v>0.0165862</v>
       </c>
     </row>
   </sheetData>
@@ -992,25 +1007,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1033,7 +1048,7 @@
         <v>0.07257142857142861</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2">
         <v>0.004524</v>
@@ -1059,7 +1074,7 @@
         <v>0.145142857142857</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3">
         <v>0.006048</v>
@@ -1085,7 +1100,7 @@
         <v>0.217714285714286</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4">
         <v>0.0164112</v>
@@ -1140,25 +1155,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1181,7 +1196,7 @@
         <v>0.06096</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2">
         <v>0.0048288</v>
@@ -1207,7 +1222,7 @@
         <v>0.12192</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3">
         <v>0.0072672</v>
@@ -1233,7 +1248,7 @@
         <v>0.18288</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4">
         <v>0.0173256</v>
@@ -1288,22 +1303,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1320,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F2">
         <v>60.01</v>
@@ -1340,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F3">
         <v>15.01</v>
@@ -1359,6 +1374,12 @@
       <c r="D4">
         <v>0</v>
       </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
@@ -1373,6 +1394,12 @@
       <c r="D5">
         <v>0</v>
       </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
@@ -1386,6 +1413,12 @@
       </c>
       <c r="D6">
         <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1401,6 +1434,12 @@
       <c r="D7">
         <v>0</v>
       </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
@@ -1415,6 +1454,12 @@
       <c r="D8">
         <v>0</v>
       </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
@@ -1429,6 +1474,12 @@
       <c r="D9">
         <v>0</v>
       </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
@@ -1443,6 +1494,12 @@
       <c r="D10">
         <v>0</v>
       </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
@@ -1457,6 +1514,12 @@
       <c r="D11">
         <v>0</v>
       </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1">
@@ -1471,6 +1534,12 @@
       <c r="D12">
         <v>0</v>
       </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1">
@@ -1485,6 +1554,12 @@
       <c r="D13">
         <v>0</v>
       </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1">
@@ -1808,7 +1883,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F36">
         <v>60</v>
@@ -1954,10 +2029,10 @@
         <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F46">
-        <v>20.0073922830283</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2185,22 +2260,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>